<commit_message>
Working version with better heatmap
</commit_message>
<xml_diff>
--- a/data/summary.xlsx
+++ b/data/summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\Git\VitaTracer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97ED43C6-9A13-4615-B498-DF0DC41733DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97077C2-04EC-4297-8DC0-936800C09FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5FE37573-B430-462E-8B71-BEB2CD0D5C54}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="143">
   <si>
     <t>Min</t>
   </si>
@@ -464,6 +464,9 @@
   </si>
   <si>
     <t>Glomerular filtration rate (GFR) via CDK EPI</t>
+  </si>
+  <si>
+    <t>2023/12/27</t>
   </si>
 </sst>
 </file>
@@ -886,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A46A3802-283E-4E98-BCAF-1BECEA2B901B}">
-  <dimension ref="A1:L289"/>
+  <dimension ref="A1:L290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C197" sqref="C197"/>
+    <sheetView tabSelected="1" topLeftCell="A256" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3941,13 +3944,13 @@
         <v>4</v>
       </c>
       <c r="F117" s="3">
-        <v>3.76</v>
+        <v>20</v>
       </c>
       <c r="G117" s="3">
         <v>11</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>5</v>
+        <v>142</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -3958,22 +3961,22 @@
         <v>63</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="E118" s="3">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F118" s="3">
-        <v>32.200000000000003</v>
+        <v>3.76</v>
       </c>
       <c r="G118" s="3">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="H118" s="2" t="s">
-        <v>126</v>
+        <v>5</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -3993,13 +3996,13 @@
         <v>20</v>
       </c>
       <c r="F119" s="3">
-        <v>34.4</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="G119" s="3">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H119" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -4016,16 +4019,16 @@
         <v>7</v>
       </c>
       <c r="E120" s="3">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F120" s="3">
-        <v>36.4</v>
+        <v>34.4</v>
       </c>
       <c r="G120" s="3">
         <v>50</v>
       </c>
       <c r="H120" s="2" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -4038,20 +4041,20 @@
       <c r="C121" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D121" s="2" t="s">
+      <c r="D121" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E121" s="3">
         <v>15</v>
       </c>
       <c r="F121" s="3">
-        <v>34.1</v>
+        <v>36.4</v>
       </c>
       <c r="G121" s="3">
         <v>50</v>
       </c>
       <c r="H121" s="2" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -4064,20 +4067,20 @@
       <c r="C122" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D122" s="1" t="s">
+      <c r="D122" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E122" s="3">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F122" s="3">
-        <v>33.4</v>
+        <v>34.1</v>
       </c>
       <c r="G122" s="3">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="H122" s="2" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -4094,16 +4097,16 @@
         <v>7</v>
       </c>
       <c r="E123" s="3">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F123" s="3">
-        <v>40.4</v>
+        <v>33.4</v>
       </c>
       <c r="G123" s="3">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -4117,19 +4120,19 @@
         <v>13</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="E124" s="3">
-        <v>0.84</v>
+        <v>16</v>
       </c>
       <c r="F124" s="3">
-        <v>1.3846000000000001</v>
+        <v>40.4</v>
       </c>
       <c r="G124" s="3">
-        <v>5.1749999999999998</v>
+        <v>45</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>126</v>
+        <v>5</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -4146,16 +4149,16 @@
         <v>49</v>
       </c>
       <c r="E125" s="3">
-        <v>1.2</v>
+        <v>0.84</v>
       </c>
       <c r="F125" s="3">
-        <v>1.3</v>
+        <v>1.3846000000000001</v>
       </c>
       <c r="G125" s="3">
-        <v>3.5</v>
+        <v>5.1749999999999998</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -4172,16 +4175,16 @@
         <v>49</v>
       </c>
       <c r="E126" s="3">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="F126" s="3">
-        <v>1.45</v>
+        <v>1.3</v>
       </c>
       <c r="G126" s="3">
-        <v>4.8</v>
+        <v>3.5</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -4201,13 +4204,13 @@
         <v>1.5</v>
       </c>
       <c r="F127" s="3">
-        <v>1.5</v>
+        <v>1.45</v>
       </c>
       <c r="G127" s="3">
         <v>4.8</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -4224,16 +4227,16 @@
         <v>49</v>
       </c>
       <c r="E128" s="3">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="F128" s="3">
-        <v>1.1000000000000001</v>
+        <v>1.5</v>
       </c>
       <c r="G128" s="3">
-        <v>4</v>
+        <v>4.8</v>
       </c>
       <c r="H128" s="2" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -4250,16 +4253,16 @@
         <v>49</v>
       </c>
       <c r="E129" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F129" s="3">
-        <v>1.5189999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G129" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H129" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -4270,22 +4273,22 @@
         <v>63</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="E130" s="3">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="F130" s="3">
-        <v>6.7</v>
+        <v>1.5189999999999999</v>
       </c>
       <c r="G130" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H130" s="2" t="s">
-        <v>126</v>
+        <v>5</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -4302,16 +4305,16 @@
         <v>7</v>
       </c>
       <c r="E131" s="3">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="F131" s="3">
-        <v>7.9</v>
+        <v>6.7</v>
       </c>
       <c r="G131" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H131" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -4328,16 +4331,16 @@
         <v>7</v>
       </c>
       <c r="E132" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F132" s="3">
-        <v>5.0999999999999996</v>
+        <v>7.9</v>
       </c>
       <c r="G132" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H132" s="2" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -4350,20 +4353,20 @@
       <c r="C133" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D133" s="2" t="s">
+      <c r="D133" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E133" s="3">
         <v>1</v>
       </c>
       <c r="F133" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="G133" s="3">
         <v>10</v>
       </c>
       <c r="H133" s="2" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
@@ -4376,20 +4379,20 @@
       <c r="C134" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D134" s="1" t="s">
+      <c r="D134" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E134" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F134" s="3">
-        <v>9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="G134" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H134" s="2" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -4415,7 +4418,7 @@
         <v>12</v>
       </c>
       <c r="H135" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -4429,19 +4432,19 @@
         <v>12</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="E136" s="3">
-        <v>4.2000000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="F136" s="3">
-        <v>0.2281</v>
+        <v>9</v>
       </c>
       <c r="G136" s="3">
-        <v>0.95</v>
+        <v>12</v>
       </c>
       <c r="H136" s="2" t="s">
-        <v>126</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -4458,16 +4461,16 @@
         <v>49</v>
       </c>
       <c r="E137" s="3">
-        <v>0.1</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="F137" s="3">
-        <v>0.3</v>
+        <v>0.2281</v>
       </c>
       <c r="G137" s="3">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="H137" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -4484,16 +4487,16 @@
         <v>49</v>
       </c>
       <c r="E138" s="3">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="F138" s="3">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="G138" s="3">
-        <v>0.92</v>
+        <v>1</v>
       </c>
       <c r="H138" s="2" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -4519,7 +4522,7 @@
         <v>0.92</v>
       </c>
       <c r="H139" s="2" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -4536,16 +4539,16 @@
         <v>49</v>
       </c>
       <c r="E140" s="3">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="F140" s="3">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="G140" s="3">
-        <v>1.2</v>
+        <v>0.92</v>
       </c>
       <c r="H140" s="2" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -4562,16 +4565,16 @@
         <v>49</v>
       </c>
       <c r="E141" s="3">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F141" s="3">
-        <v>0.33800000000000002</v>
+        <v>0.3</v>
       </c>
       <c r="G141" s="3">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="H141" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
@@ -4582,22 +4585,22 @@
         <v>63</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="E142" s="3">
-        <v>45</v>
+        <v>0.2</v>
       </c>
       <c r="F142" s="3">
-        <v>58.8</v>
+        <v>0.33800000000000002</v>
       </c>
       <c r="G142" s="3">
-        <v>75</v>
+        <v>1</v>
       </c>
       <c r="H142" s="2" t="s">
-        <v>126</v>
+        <v>5</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -4614,16 +4617,16 @@
         <v>7</v>
       </c>
       <c r="E143" s="3">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F143" s="3">
-        <v>54</v>
+        <v>58.8</v>
       </c>
       <c r="G143" s="3">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H143" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
@@ -4640,16 +4643,16 @@
         <v>7</v>
       </c>
       <c r="E144" s="3">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F144" s="3">
-        <v>51.4</v>
+        <v>54</v>
       </c>
       <c r="G144" s="3">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="H144" s="2" t="s">
-        <v>67</v>
+        <v>122</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -4666,16 +4669,16 @@
         <v>7</v>
       </c>
       <c r="E145" s="3">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="F145" s="3">
-        <v>48</v>
+        <v>51.4</v>
       </c>
       <c r="G145" s="3">
         <v>70</v>
       </c>
       <c r="H145" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
@@ -4689,19 +4692,19 @@
         <v>14</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="E146" s="3">
-        <v>1.89</v>
+        <v>35</v>
       </c>
       <c r="F146" s="3">
-        <v>2.5284</v>
+        <v>48</v>
       </c>
       <c r="G146" s="3">
-        <v>8.5749999999999993</v>
+        <v>70</v>
       </c>
       <c r="H146" s="2" t="s">
-        <v>126</v>
+        <v>5</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
@@ -4718,16 +4721,16 @@
         <v>49</v>
       </c>
       <c r="E147" s="3">
-        <v>2</v>
+        <v>1.89</v>
       </c>
       <c r="F147" s="3">
-        <v>2.1</v>
+        <v>2.5284</v>
       </c>
       <c r="G147" s="3">
-        <v>7</v>
+        <v>8.5749999999999993</v>
       </c>
       <c r="H147" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
@@ -4747,13 +4750,13 @@
         <v>2</v>
       </c>
       <c r="F148" s="3">
-        <v>1.7</v>
+        <v>2.1</v>
       </c>
       <c r="G148" s="3">
-        <v>7.5</v>
+        <v>7</v>
       </c>
       <c r="H148" s="2" t="s">
-        <v>67</v>
+        <v>122</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
@@ -4770,16 +4773,16 @@
         <v>49</v>
       </c>
       <c r="E149" s="3">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="F149" s="3">
-        <v>1.8049999999999999</v>
+        <v>1.7</v>
       </c>
       <c r="G149" s="3">
         <v>7.5</v>
       </c>
       <c r="H149" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -4787,22 +4790,22 @@
         <v>60</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>107</v>
+        <v>63</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E150" s="3">
-        <v>1.58</v>
+        <v>1.8</v>
       </c>
       <c r="F150" s="3">
-        <v>2.81</v>
+        <v>1.8049999999999999</v>
       </c>
       <c r="G150" s="3">
-        <v>3.91</v>
+        <v>7.5</v>
       </c>
       <c r="H150" s="2" t="s">
         <v>5</v>
@@ -4816,19 +4819,19 @@
         <v>107</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E151" s="3">
-        <v>0.71</v>
+        <v>1.58</v>
       </c>
       <c r="F151" s="3">
-        <v>1.2</v>
+        <v>2.81</v>
       </c>
       <c r="G151" s="3">
-        <v>1.85</v>
+        <v>3.91</v>
       </c>
       <c r="H151" s="2" t="s">
         <v>5</v>
@@ -4848,16 +4851,16 @@
         <v>47</v>
       </c>
       <c r="E152" s="3">
-        <v>0.69920000000000004</v>
+        <v>0.71</v>
       </c>
       <c r="F152" s="3">
-        <v>1.0566</v>
+        <v>1.2</v>
       </c>
       <c r="G152" s="3">
-        <v>1.4761</v>
+        <v>1.85</v>
       </c>
       <c r="H152" s="2" t="s">
-        <v>91</v>
+        <v>5</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -4868,22 +4871,22 @@
         <v>107</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="E153" s="3">
-        <v>0.47</v>
+        <v>0.69920000000000004</v>
       </c>
       <c r="F153" s="3">
-        <v>7.16</v>
+        <v>1.0566</v>
       </c>
       <c r="G153" s="3">
-        <v>9.8000000000000007</v>
+        <v>1.4761</v>
       </c>
       <c r="H153" s="2" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -4894,22 +4897,22 @@
         <v>107</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>98</v>
+        <v>19</v>
       </c>
       <c r="E154" s="3">
-        <v>0.55000000000000004</v>
+        <v>0.47</v>
       </c>
       <c r="F154" s="3">
-        <v>1.984</v>
+        <v>7.16</v>
       </c>
       <c r="G154" s="3">
-        <v>4.78</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="H154" s="2" t="s">
-        <v>122</v>
+        <v>5</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
@@ -4926,16 +4929,16 @@
         <v>98</v>
       </c>
       <c r="E155" s="3">
-        <v>0.3</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F155" s="3">
-        <v>0.67</v>
+        <v>1.984</v>
       </c>
       <c r="G155" s="3">
-        <v>4.3</v>
+        <v>4.78</v>
       </c>
       <c r="H155" s="2" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
@@ -4955,13 +4958,13 @@
         <v>0.3</v>
       </c>
       <c r="F156" s="3">
-        <v>0.53</v>
+        <v>0.67</v>
       </c>
       <c r="G156" s="3">
         <v>4.3</v>
       </c>
       <c r="H156" s="2" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
@@ -4978,16 +4981,16 @@
         <v>98</v>
       </c>
       <c r="E157" s="3">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="F157" s="3">
-        <v>0.72</v>
+        <v>0.53</v>
       </c>
       <c r="G157" s="3">
-        <v>3.7</v>
+        <v>4.3</v>
       </c>
       <c r="H157" s="2" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
@@ -4995,25 +4998,25 @@
         <v>60</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="E158" s="3">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="F158" s="3">
-        <v>2</v>
+        <v>0.72</v>
       </c>
       <c r="G158" s="3">
-        <v>12</v>
+        <v>3.7</v>
       </c>
       <c r="H158" s="2" t="s">
-        <v>85</v>
+        <v>5</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -5024,22 +5027,22 @@
         <v>103</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>89</v>
+        <v>35</v>
       </c>
       <c r="E159" s="3">
         <v>0</v>
       </c>
       <c r="F159" s="3">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="G159" s="3">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H159" s="2" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -5059,13 +5062,13 @@
         <v>0</v>
       </c>
       <c r="F160" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G160" s="3">
         <v>5</v>
       </c>
       <c r="H160" s="2" t="s">
-        <v>111</v>
+        <v>5</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
@@ -5078,20 +5081,20 @@
       <c r="C161" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D161" s="2" t="s">
+      <c r="D161" s="1" t="s">
         <v>89</v>
       </c>
       <c r="E161" s="3">
         <v>0</v>
       </c>
       <c r="F161" s="3">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G161" s="3">
         <v>5</v>
       </c>
       <c r="H161" s="2" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
@@ -5104,20 +5107,20 @@
       <c r="C162" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D162" s="1" t="s">
+      <c r="D162" s="2" t="s">
         <v>89</v>
       </c>
       <c r="E162" s="3">
         <v>0</v>
       </c>
       <c r="F162" s="3">
-        <v>0.61</v>
+        <v>0.4</v>
       </c>
       <c r="G162" s="3">
         <v>5</v>
       </c>
       <c r="H162" s="2" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
@@ -5125,25 +5128,25 @@
         <v>60</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>141</v>
+        <v>40</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="E163" s="3">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="F163" s="3">
-        <v>100</v>
-      </c>
-      <c r="G163" s="3" t="s">
-        <v>41</v>
+        <v>0.61</v>
+      </c>
+      <c r="G163" s="3">
+        <v>5</v>
       </c>
       <c r="H163" s="2" t="s">
-        <v>122</v>
+        <v>85</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
@@ -5163,13 +5166,13 @@
         <v>90</v>
       </c>
       <c r="F164" s="3">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="G164" s="3" t="s">
         <v>41</v>
       </c>
       <c r="H164" s="2" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
@@ -5189,13 +5192,13 @@
         <v>90</v>
       </c>
       <c r="F165" s="3">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="G165" s="3" t="s">
         <v>41</v>
       </c>
       <c r="H165" s="2" t="s">
-        <v>67</v>
+        <v>111</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
@@ -5206,22 +5209,22 @@
         <v>139</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>26</v>
+        <v>141</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="E166" s="3">
-        <v>0.8</v>
+        <v>90</v>
       </c>
       <c r="F166" s="3">
-        <v>1.03</v>
-      </c>
-      <c r="G166" s="3">
-        <v>1.25</v>
+        <v>124</v>
+      </c>
+      <c r="G166" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="H166" s="2" t="s">
-        <v>126</v>
+        <v>67</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
@@ -5238,16 +5241,16 @@
         <v>33</v>
       </c>
       <c r="E167" s="3">
-        <v>0.67</v>
+        <v>0.8</v>
       </c>
       <c r="F167" s="3">
-        <v>0.99</v>
+        <v>1.03</v>
       </c>
       <c r="G167" s="3">
-        <v>1.17</v>
+        <v>1.25</v>
       </c>
       <c r="H167" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
@@ -5264,16 +5267,16 @@
         <v>33</v>
       </c>
       <c r="E168" s="3">
-        <v>0.73</v>
+        <v>0.67</v>
       </c>
       <c r="F168" s="3">
-        <v>0.8</v>
+        <v>0.99</v>
       </c>
       <c r="G168" s="3">
-        <v>1.18</v>
+        <v>1.17</v>
       </c>
       <c r="H168" s="2" t="s">
-        <v>5</v>
+        <v>122</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
@@ -5290,16 +5293,16 @@
         <v>33</v>
       </c>
       <c r="E169" s="3">
-        <v>0.59889999999999999</v>
+        <v>0.73</v>
       </c>
       <c r="F169" s="3">
-        <v>1.0283</v>
+        <v>0.8</v>
       </c>
       <c r="G169" s="3">
-        <v>1.2429999999999999</v>
+        <v>1.18</v>
       </c>
       <c r="H169" s="2" t="s">
-        <v>111</v>
+        <v>5</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
@@ -5316,16 +5319,16 @@
         <v>33</v>
       </c>
       <c r="E170" s="3">
-        <v>0.49719999999999998</v>
+        <v>0.59889999999999999</v>
       </c>
       <c r="F170" s="3">
-        <v>0.96049999999999991</v>
+        <v>1.0283</v>
       </c>
       <c r="G170" s="3">
-        <v>1.1752</v>
+        <v>1.2429999999999999</v>
       </c>
       <c r="H170" s="2" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
@@ -5342,16 +5345,16 @@
         <v>33</v>
       </c>
       <c r="E171" s="3">
-        <v>0.59889999999999999</v>
+        <v>0.49719999999999998</v>
       </c>
       <c r="F171" s="3">
-        <v>0.73449999999999993</v>
+        <v>0.96049999999999991</v>
       </c>
       <c r="G171" s="3">
-        <v>1.2994999999999999</v>
+        <v>1.1752</v>
       </c>
       <c r="H171" s="2" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
@@ -5359,25 +5362,25 @@
         <v>60</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D172" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E172" s="3">
-        <v>130</v>
+        <v>0.59889999999999999</v>
       </c>
       <c r="F172" s="3">
-        <v>159</v>
+        <v>0.73449999999999993</v>
       </c>
       <c r="G172" s="3">
-        <v>220</v>
+        <v>1.2994999999999999</v>
       </c>
       <c r="H172" s="2" t="s">
-        <v>126</v>
+        <v>67</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
@@ -5394,16 +5397,16 @@
         <v>33</v>
       </c>
       <c r="E173" s="3">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F173" s="3">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="G173" s="3">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="H173" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
@@ -5420,16 +5423,16 @@
         <v>33</v>
       </c>
       <c r="E174" s="3">
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="F174" s="3">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="G174" s="3">
-        <v>200</v>
+        <v>240</v>
       </c>
       <c r="H174" s="2" t="s">
-        <v>5</v>
+        <v>122</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
@@ -5449,13 +5452,13 @@
         <v>0</v>
       </c>
       <c r="F175" s="3">
-        <v>149.24690000000001</v>
+        <v>120</v>
       </c>
       <c r="G175" s="3">
-        <v>212.65750000000003</v>
+        <v>200</v>
       </c>
       <c r="H175" s="2" t="s">
-        <v>111</v>
+        <v>5</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
@@ -5475,13 +5478,13 @@
         <v>0</v>
       </c>
       <c r="F176" s="3">
-        <v>111.74185000000003</v>
+        <v>149.24690000000001</v>
       </c>
       <c r="G176" s="3">
         <v>212.65750000000003</v>
       </c>
       <c r="H176" s="2" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
@@ -5501,13 +5504,13 @@
         <v>0</v>
       </c>
       <c r="F177" s="3">
-        <v>150.79350000000002</v>
+        <v>111.74185000000003</v>
       </c>
       <c r="G177" s="3">
-        <v>193.32500000000005</v>
+        <v>212.65750000000003</v>
       </c>
       <c r="H177" s="2" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
@@ -5518,22 +5521,22 @@
         <v>105</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D178" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E178" s="3">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="F178" s="3">
-        <v>52</v>
-      </c>
-      <c r="G178" s="3" t="s">
-        <v>41</v>
+        <v>150.79350000000002</v>
+      </c>
+      <c r="G178" s="3">
+        <v>193.32500000000005</v>
       </c>
       <c r="H178" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
@@ -5550,16 +5553,16 @@
         <v>33</v>
       </c>
       <c r="E179" s="3">
-        <v>38.665000000000006</v>
+        <v>40</v>
       </c>
       <c r="F179" s="3">
-        <v>40.211600000000011</v>
+        <v>52</v>
       </c>
       <c r="G179" s="3" t="s">
         <v>41</v>
       </c>
       <c r="H179" s="2" t="s">
-        <v>111</v>
+        <v>5</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
@@ -5579,13 +5582,13 @@
         <v>38.665000000000006</v>
       </c>
       <c r="F180" s="3">
-        <v>40.598250000000007</v>
+        <v>40.211600000000011</v>
       </c>
       <c r="G180" s="3" t="s">
         <v>41</v>
       </c>
       <c r="H180" s="2" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
@@ -5605,13 +5608,13 @@
         <v>38.665000000000006</v>
       </c>
       <c r="F181" s="3">
-        <v>50.264500000000012</v>
+        <v>40.598250000000007</v>
       </c>
       <c r="G181" s="3" t="s">
         <v>41</v>
       </c>
       <c r="H181" s="2" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
@@ -5622,22 +5625,22 @@
         <v>105</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D182" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E182" s="3">
-        <v>0</v>
+        <v>38.665000000000006</v>
       </c>
       <c r="F182" s="3">
-        <v>59</v>
-      </c>
-      <c r="G182" s="3">
-        <v>130</v>
+        <v>50.264500000000012</v>
+      </c>
+      <c r="G182" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="H182" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
@@ -5657,13 +5660,13 @@
         <v>0</v>
       </c>
       <c r="F183" s="3">
-        <v>98.982400000000013</v>
+        <v>59</v>
       </c>
       <c r="G183" s="3">
-        <v>115.99500000000002</v>
+        <v>130</v>
       </c>
       <c r="H183" s="2" t="s">
-        <v>111</v>
+        <v>5</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
@@ -5683,13 +5686,13 @@
         <v>0</v>
       </c>
       <c r="F184" s="3">
-        <v>63.410600000000009</v>
+        <v>98.982400000000013</v>
       </c>
       <c r="G184" s="3">
         <v>115.99500000000002</v>
       </c>
       <c r="H184" s="2" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
@@ -5709,13 +5712,13 @@
         <v>0</v>
       </c>
       <c r="F185" s="3">
-        <v>88.929500000000004</v>
+        <v>63.410600000000009</v>
       </c>
       <c r="G185" s="3">
-        <v>112.12850000000002</v>
+        <v>115.99500000000002</v>
       </c>
       <c r="H185" s="2" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.25">
@@ -5726,22 +5729,22 @@
         <v>105</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D186" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E186" s="3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F186" s="3">
-        <v>55</v>
+        <v>88.929500000000004</v>
       </c>
       <c r="G186" s="3">
-        <v>185</v>
+        <v>112.12850000000002</v>
       </c>
       <c r="H186" s="2" t="s">
-        <v>126</v>
+        <v>67</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
@@ -5758,16 +5761,16 @@
         <v>33</v>
       </c>
       <c r="E187" s="3">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="F187" s="3">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="G187" s="3">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="H187" s="2" t="s">
-        <v>5</v>
+        <v>126</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
@@ -5787,13 +5790,13 @@
         <v>0</v>
       </c>
       <c r="F188" s="3">
-        <v>50.444999999999993</v>
+        <v>47</v>
       </c>
       <c r="G188" s="3">
-        <v>150.44999999999999</v>
+        <v>150</v>
       </c>
       <c r="H188" s="2" t="s">
-        <v>111</v>
+        <v>5</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.25">
@@ -5813,13 +5816,13 @@
         <v>0</v>
       </c>
       <c r="F189" s="3">
-        <v>38.94</v>
+        <v>50.444999999999993</v>
       </c>
       <c r="G189" s="3">
         <v>150.44999999999999</v>
       </c>
       <c r="H189" s="2" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
@@ -5839,13 +5842,13 @@
         <v>0</v>
       </c>
       <c r="F190" s="3">
-        <v>44.25</v>
+        <v>38.94</v>
       </c>
       <c r="G190" s="3">
         <v>150.44999999999999</v>
       </c>
       <c r="H190" s="2" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
@@ -5853,22 +5856,22 @@
         <v>60</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="E191" s="3">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F191" s="3">
-        <v>278</v>
+        <v>44.25</v>
       </c>
       <c r="G191" s="3">
-        <v>285</v>
+        <v>150.44999999999999</v>
       </c>
       <c r="H191" s="2" t="s">
         <v>67</v>
@@ -5882,22 +5885,22 @@
         <v>82</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="E192" s="3">
-        <v>65</v>
+        <v>200</v>
       </c>
       <c r="F192" s="3">
-        <v>84</v>
+        <v>278</v>
       </c>
       <c r="G192" s="3">
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="H192" s="2" t="s">
-        <v>126</v>
+        <v>67</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
@@ -5914,16 +5917,16 @@
         <v>33</v>
       </c>
       <c r="E193" s="3">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F193" s="3">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="G193" s="3">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H193" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
@@ -5940,16 +5943,16 @@
         <v>33</v>
       </c>
       <c r="E194" s="3">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="F194" s="3">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="G194" s="3">
         <v>110</v>
       </c>
       <c r="H194" s="2" t="s">
-        <v>5</v>
+        <v>122</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
@@ -5966,16 +5969,16 @@
         <v>33</v>
       </c>
       <c r="E195" s="3">
-        <v>70.262399999999985</v>
+        <v>60</v>
       </c>
       <c r="F195" s="3">
-        <v>88.278400000000005</v>
+        <v>88</v>
       </c>
       <c r="G195" s="3">
-        <v>109.89759999999998</v>
+        <v>110</v>
       </c>
       <c r="H195" s="2" t="s">
-        <v>111</v>
+        <v>5</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
@@ -5995,13 +5998,13 @@
         <v>70.262399999999985</v>
       </c>
       <c r="F196" s="3">
-        <v>75.667199999999994</v>
+        <v>88.278400000000005</v>
       </c>
       <c r="G196" s="3">
         <v>109.89759999999998</v>
       </c>
       <c r="H196" s="2" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
@@ -6009,25 +6012,25 @@
         <v>60</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D197" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E197" s="3">
-        <v>8.1999999999999993</v>
+        <v>70.262399999999985</v>
       </c>
       <c r="F197" s="3">
-        <v>9.6</v>
+        <v>75.667199999999994</v>
       </c>
       <c r="G197" s="3">
-        <v>10.6</v>
+        <v>109.89759999999998</v>
       </c>
       <c r="H197" s="2" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.25">
@@ -6044,16 +6047,16 @@
         <v>33</v>
       </c>
       <c r="E198" s="3">
-        <v>8.4163800000000002</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="F198" s="3">
-        <v>9.1377839999999981</v>
+        <v>9.6</v>
       </c>
       <c r="G198" s="3">
-        <v>10.42028</v>
+        <v>10.6</v>
       </c>
       <c r="H198" s="2" t="s">
-        <v>91</v>
+        <v>5</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.25">
@@ -6073,13 +6076,13 @@
         <v>8.4163800000000002</v>
       </c>
       <c r="F199" s="3">
-        <v>9.899265999999999</v>
+        <v>9.1377839999999981</v>
       </c>
       <c r="G199" s="3">
-        <v>10.620669999999999</v>
+        <v>10.42028</v>
       </c>
       <c r="H199" s="2" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.25">
@@ -6090,22 +6093,22 @@
         <v>106</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E200" s="3">
-        <v>95</v>
+        <v>8.4163800000000002</v>
       </c>
       <c r="F200" s="3">
-        <v>97</v>
+        <v>9.899265999999999</v>
       </c>
       <c r="G200" s="3">
-        <v>110</v>
+        <v>10.620669999999999</v>
       </c>
       <c r="H200" s="2" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.25">
@@ -6118,20 +6121,20 @@
       <c r="C201" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D201" s="2" t="s">
+      <c r="D201" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E201" s="3">
         <v>95</v>
       </c>
       <c r="F201" s="3">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G201" s="3">
         <v>110</v>
       </c>
       <c r="H201" s="2" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.25">
@@ -6142,22 +6145,22 @@
         <v>106</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D202" s="1" t="s">
-        <v>118</v>
+        <v>90</v>
+      </c>
+      <c r="D202" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="E202" s="3">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="F202" s="3">
-        <v>109.7</v>
+        <v>96</v>
       </c>
       <c r="G202" s="3">
-        <v>350</v>
+        <v>110</v>
       </c>
       <c r="H202" s="2" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.25">
@@ -6177,13 +6180,13 @@
         <v>30</v>
       </c>
       <c r="F203" s="3">
-        <v>86.2</v>
+        <v>109.7</v>
       </c>
       <c r="G203" s="3">
         <v>350</v>
       </c>
       <c r="H203" s="2" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.25">
@@ -6200,16 +6203,16 @@
         <v>118</v>
       </c>
       <c r="E204" s="3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F204" s="3">
-        <v>92</v>
+        <v>86.2</v>
       </c>
       <c r="G204" s="3">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="H204" s="2" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.25">
@@ -6226,16 +6229,16 @@
         <v>118</v>
       </c>
       <c r="E205" s="3">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="F205" s="3">
-        <v>120.6</v>
+        <v>92</v>
       </c>
       <c r="G205" s="3">
         <v>300</v>
       </c>
       <c r="H205" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.25">
@@ -6246,19 +6249,19 @@
         <v>106</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="E206" s="3">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="F206" s="3">
-        <v>96</v>
+        <v>120.6</v>
       </c>
       <c r="G206" s="3">
-        <v>160</v>
+        <v>300</v>
       </c>
       <c r="H206" s="2" t="s">
         <v>5</v>
@@ -6278,16 +6281,16 @@
         <v>51</v>
       </c>
       <c r="E207" s="3">
-        <v>61.429500000000004</v>
+        <v>59</v>
       </c>
       <c r="F207" s="3">
-        <v>86.001300000000001</v>
+        <v>96</v>
       </c>
       <c r="G207" s="3">
-        <v>156.36600000000001</v>
+        <v>160</v>
       </c>
       <c r="H207" s="2" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.25">
@@ -6298,22 +6301,22 @@
         <v>106</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E208" s="3">
-        <v>0.65</v>
+        <v>61.429500000000004</v>
       </c>
       <c r="F208" s="3">
-        <v>0.84</v>
+        <v>86.001300000000001</v>
       </c>
       <c r="G208" s="3">
-        <v>1.05</v>
+        <v>156.36600000000001</v>
       </c>
       <c r="H208" s="2" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.25">
@@ -6326,20 +6329,20 @@
       <c r="C209" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D209" s="2" t="s">
+      <c r="D209" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E209" s="3">
         <v>0.65</v>
       </c>
       <c r="F209" s="3">
-        <v>0.91</v>
+        <v>0.84</v>
       </c>
       <c r="G209" s="3">
         <v>1.05</v>
       </c>
       <c r="H209" s="2" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.25">
@@ -6352,20 +6355,20 @@
       <c r="C210" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D210" s="1" t="s">
+      <c r="D210" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E210" s="3">
-        <v>0.66</v>
+        <v>0.65</v>
       </c>
       <c r="F210" s="3">
-        <v>0.9</v>
+        <v>0.91</v>
       </c>
       <c r="G210" s="3">
-        <v>1.07</v>
+        <v>1.05</v>
       </c>
       <c r="H210" s="2" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.25">
@@ -6376,19 +6379,19 @@
         <v>106</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E211" s="3">
-        <v>2.5</v>
+        <v>0.66</v>
       </c>
       <c r="F211" s="3">
-        <v>4.5</v>
+        <v>0.9</v>
       </c>
       <c r="G211" s="3">
-        <v>5</v>
+        <v>1.07</v>
       </c>
       <c r="H211" s="2" t="s">
         <v>5</v>
@@ -6408,16 +6411,16 @@
         <v>33</v>
       </c>
       <c r="E212" s="3">
-        <v>2.6970000000000001</v>
+        <v>2.5</v>
       </c>
       <c r="F212" s="3">
-        <v>3.7509999999999999</v>
+        <v>4.5</v>
       </c>
       <c r="G212" s="3">
-        <v>4.4950000000000001</v>
+        <v>5</v>
       </c>
       <c r="H212" s="2" t="s">
-        <v>91</v>
+        <v>5</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
@@ -6437,13 +6440,13 @@
         <v>2.6970000000000001</v>
       </c>
       <c r="F213" s="3">
-        <v>3.6269999999999998</v>
+        <v>3.7509999999999999</v>
       </c>
       <c r="G213" s="3">
         <v>4.4950000000000001</v>
       </c>
       <c r="H213" s="2" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.25">
@@ -6454,22 +6457,22 @@
         <v>106</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E214" s="3">
-        <v>3.5</v>
+        <v>2.6970000000000001</v>
       </c>
       <c r="F214" s="3">
-        <v>4.3899999999999997</v>
+        <v>3.6269999999999998</v>
       </c>
       <c r="G214" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.4950000000000001</v>
       </c>
       <c r="H214" s="2" t="s">
-        <v>122</v>
+        <v>67</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
@@ -6489,13 +6492,13 @@
         <v>3.5</v>
       </c>
       <c r="F215" s="3">
-        <v>4</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="G215" s="3">
-        <v>5.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="H215" s="2" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.25">
@@ -6512,16 +6515,16 @@
         <v>35</v>
       </c>
       <c r="E216" s="3">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="F216" s="3">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="G216" s="3">
-        <v>4.8</v>
+        <v>5.3</v>
       </c>
       <c r="H216" s="2" t="s">
-        <v>67</v>
+        <v>111</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.25">
@@ -6538,16 +6541,16 @@
         <v>35</v>
       </c>
       <c r="E217" s="3">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="F217" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="G217" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.8</v>
       </c>
       <c r="H217" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.25">
@@ -6558,22 +6561,22 @@
         <v>106</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D218" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E218" s="3">
-        <v>136</v>
+        <v>3.5</v>
       </c>
       <c r="F218" s="3">
-        <v>140.19999999999999</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="G218" s="3">
-        <v>146</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="H218" s="2" t="s">
-        <v>122</v>
+        <v>5</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
@@ -6590,16 +6593,16 @@
         <v>35</v>
       </c>
       <c r="E219" s="3">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F219" s="3">
-        <v>140</v>
+        <v>140.19999999999999</v>
       </c>
       <c r="G219" s="3">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H219" s="2" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
@@ -6612,20 +6615,20 @@
       <c r="C220" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D220" s="2" t="s">
+      <c r="D220" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E220" s="3">
         <v>135</v>
       </c>
       <c r="F220" s="3">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G220" s="3">
         <v>145</v>
       </c>
       <c r="H220" s="2" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
@@ -6638,20 +6641,20 @@
       <c r="C221" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D221" s="1" t="s">
+      <c r="D221" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E221" s="3">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F221" s="3">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G221" s="3">
         <v>145</v>
       </c>
       <c r="H221" s="2" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
@@ -6668,16 +6671,16 @@
         <v>35</v>
       </c>
       <c r="E222" s="3">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F222" s="3">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G222" s="3">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H222" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
@@ -6685,22 +6688,22 @@
         <v>60</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E223" s="3">
-        <v>0.2</v>
+        <v>135</v>
       </c>
       <c r="F223" s="3">
-        <v>1.2</v>
+        <v>139</v>
       </c>
       <c r="G223" s="3">
-        <v>1.2</v>
+        <v>147</v>
       </c>
       <c r="H223" s="2" t="s">
         <v>5</v>
@@ -6720,16 +6723,16 @@
         <v>33</v>
       </c>
       <c r="E224" s="3">
-        <v>0.2923</v>
+        <v>0.2</v>
       </c>
       <c r="F224" s="3">
-        <v>0.99980000000000002</v>
+        <v>1.2</v>
       </c>
       <c r="G224" s="3">
-        <v>1.5201</v>
+        <v>1.2</v>
       </c>
       <c r="H224" s="2" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.25">
@@ -6740,22 +6743,22 @@
         <v>127</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="D225" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E225" s="3">
-        <v>0</v>
+        <v>0.2923</v>
       </c>
       <c r="F225" s="3">
-        <v>0.33</v>
+        <v>0.99980000000000002</v>
       </c>
       <c r="G225" s="3">
-        <v>0.3</v>
+        <v>1.5201</v>
       </c>
       <c r="H225" s="2" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.25">
@@ -6766,7 +6769,7 @@
         <v>127</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D226" s="1" t="s">
         <v>33</v>
@@ -6775,10 +6778,10 @@
         <v>0</v>
       </c>
       <c r="F226" s="3">
-        <v>0.53</v>
+        <v>0.33</v>
       </c>
       <c r="G226" s="3">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="H226" s="2" t="s">
         <v>85</v>
@@ -6792,7 +6795,7 @@
         <v>127</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D227" s="1" t="s">
         <v>33</v>
@@ -6801,10 +6804,10 @@
         <v>0</v>
       </c>
       <c r="F227" s="3">
-        <v>0.86</v>
+        <v>0.53</v>
       </c>
       <c r="G227" s="3">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="H227" s="2" t="s">
         <v>85</v>
@@ -6818,19 +6821,19 @@
         <v>127</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E228" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F228" s="3">
-        <v>15.6</v>
+        <v>0.86</v>
       </c>
       <c r="G228" s="3">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="H228" s="2" t="s">
         <v>85</v>
@@ -6850,16 +6853,16 @@
         <v>35</v>
       </c>
       <c r="E229" s="3">
-        <v>5.46</v>
+        <v>5</v>
       </c>
       <c r="F229" s="3">
-        <v>10.55</v>
+        <v>15.6</v>
       </c>
       <c r="G229" s="3">
-        <v>16.2</v>
+        <v>15</v>
       </c>
       <c r="H229" s="2" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.25">
@@ -6870,22 +6873,22 @@
         <v>127</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>135</v>
+        <v>66</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="E230" s="3">
-        <v>35</v>
+        <v>5.46</v>
       </c>
       <c r="F230" s="3">
-        <v>46</v>
+        <v>10.55</v>
       </c>
       <c r="G230" s="3">
-        <v>52</v>
+        <v>16.2</v>
       </c>
       <c r="H230" s="2" t="s">
-        <v>91</v>
+        <v>5</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.25">
@@ -6905,13 +6908,13 @@
         <v>35</v>
       </c>
       <c r="F231" s="3">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G231" s="3">
         <v>52</v>
       </c>
       <c r="H231" s="2" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.25">
@@ -6922,19 +6925,19 @@
         <v>127</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>73</v>
+        <v>135</v>
       </c>
       <c r="D232" s="1" t="s">
         <v>70</v>
       </c>
       <c r="E232" s="3">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="F232" s="3">
-        <v>25.3</v>
+        <v>47</v>
       </c>
       <c r="G232" s="3">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="H232" s="2" t="s">
         <v>67</v>
@@ -6948,22 +6951,22 @@
         <v>127</v>
       </c>
       <c r="C233" s="2" t="s">
-        <v>134</v>
+        <v>73</v>
       </c>
       <c r="D233" s="1" t="s">
         <v>70</v>
       </c>
       <c r="E233" s="3">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="F233" s="3">
-        <v>71</v>
+        <v>25.3</v>
       </c>
       <c r="G233" s="3">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="H233" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.25">
@@ -6980,16 +6983,16 @@
         <v>70</v>
       </c>
       <c r="E234" s="3">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F234" s="3">
-        <v>72.3</v>
+        <v>71</v>
       </c>
       <c r="G234" s="3">
         <v>83</v>
       </c>
       <c r="H234" s="2" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.25">
@@ -6997,25 +7000,25 @@
         <v>60</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>61</v>
+        <v>127</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>42</v>
+        <v>134</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="E235" s="3">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="F235" s="3">
-        <v>0.43</v>
+        <v>72.3</v>
       </c>
       <c r="G235" s="3">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="H235" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.25">
@@ -7023,22 +7026,22 @@
         <v>60</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>137</v>
+        <v>61</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>136</v>
+        <v>42</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E236" s="3">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F236" s="3">
-        <v>11.2</v>
+        <v>0.43</v>
       </c>
       <c r="G236" s="3">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="H236" s="2" t="s">
         <v>5</v>
@@ -7052,22 +7055,22 @@
         <v>137</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D237" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E237" s="3">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F237" s="3">
-        <v>30</v>
+        <v>11.2</v>
       </c>
       <c r="G237" s="3">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="H237" s="2" t="s">
-        <v>126</v>
+        <v>5</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.25">
@@ -7084,16 +7087,16 @@
         <v>33</v>
       </c>
       <c r="E238" s="3">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F238" s="3">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G238" s="3">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H238" s="2" t="s">
-        <v>5</v>
+        <v>126</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.25">
@@ -7110,16 +7113,16 @@
         <v>33</v>
       </c>
       <c r="E239" s="3">
-        <v>19.219200000000001</v>
+        <v>17</v>
       </c>
       <c r="F239" s="3">
-        <v>22.822800000000001</v>
+        <v>24</v>
       </c>
       <c r="G239" s="3">
-        <v>43.843800000000002</v>
+        <v>51</v>
       </c>
       <c r="H239" s="2" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.25">
@@ -7130,22 +7133,22 @@
         <v>137</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D240" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E240" s="3">
-        <v>2.5</v>
+        <v>19.219200000000001</v>
       </c>
       <c r="F240" s="3">
-        <v>4.0999999999999996</v>
+        <v>22.822800000000001</v>
       </c>
       <c r="G240" s="3">
-        <v>7.5</v>
+        <v>43.843800000000002</v>
       </c>
       <c r="H240" s="2" t="s">
-        <v>126</v>
+        <v>67</v>
       </c>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.25">
@@ -7162,16 +7165,16 @@
         <v>33</v>
       </c>
       <c r="E241" s="3">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="F241" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="G241" s="3">
-        <v>7.2</v>
+        <v>7.5</v>
       </c>
       <c r="H241" s="2" t="s">
-        <v>5</v>
+        <v>126</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.25">
@@ -7191,13 +7194,13 @@
         <v>3.5</v>
       </c>
       <c r="F242" s="3">
-        <v>4.9055999999999997</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="G242" s="3">
-        <v>7.0559999999999992</v>
+        <v>7.2</v>
       </c>
       <c r="H242" s="2" t="s">
-        <v>111</v>
+        <v>5</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.25">
@@ -7214,16 +7217,16 @@
         <v>33</v>
       </c>
       <c r="E243" s="3">
-        <v>3.5279999999999996</v>
+        <v>3.5</v>
       </c>
       <c r="F243" s="3">
-        <v>4.1495999999999995</v>
+        <v>4.9055999999999997</v>
       </c>
       <c r="G243" s="3">
         <v>7.0559999999999992</v>
       </c>
       <c r="H243" s="2" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.25">
@@ -7243,39 +7246,39 @@
         <v>3.5279999999999996</v>
       </c>
       <c r="F244" s="3">
-        <v>3.9983999999999997</v>
+        <v>4.1495999999999995</v>
       </c>
       <c r="G244" s="3">
         <v>7.0559999999999992</v>
       </c>
       <c r="H244" s="2" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>54</v>
+        <v>137</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="D245" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E245" s="3">
-        <v>0</v>
+        <v>3.5279999999999996</v>
       </c>
       <c r="F245" s="3">
-        <v>0</v>
+        <v>3.9983999999999997</v>
       </c>
       <c r="G245" s="3">
-        <v>0</v>
+        <v>7.0559999999999992</v>
       </c>
       <c r="H245" s="2" t="s">
-        <v>126</v>
+        <v>67</v>
       </c>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.25">
@@ -7301,7 +7304,7 @@
         <v>0</v>
       </c>
       <c r="H246" s="2" t="s">
-        <v>5</v>
+        <v>126</v>
       </c>
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.25">
@@ -7312,7 +7315,7 @@
         <v>54</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="D247" s="1" t="s">
         <v>33</v>
@@ -7327,7 +7330,7 @@
         <v>0</v>
       </c>
       <c r="H247" s="2" t="s">
-        <v>85</v>
+        <v>5</v>
       </c>
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.25">
@@ -7353,7 +7356,7 @@
         <v>0</v>
       </c>
       <c r="H248" s="2" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.25">
@@ -7364,22 +7367,22 @@
         <v>54</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D249" s="2" t="s">
-        <v>70</v>
+        <v>23</v>
+      </c>
+      <c r="D249" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="E249" s="3">
-        <v>1010</v>
+        <v>0</v>
       </c>
       <c r="F249" s="3">
-        <v>1020</v>
+        <v>0</v>
       </c>
       <c r="G249" s="3">
-        <v>1030</v>
+        <v>0</v>
       </c>
       <c r="H249" s="2" t="s">
-        <v>126</v>
+        <v>5</v>
       </c>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.25">
@@ -7396,16 +7399,16 @@
         <v>70</v>
       </c>
       <c r="E250" s="3">
-        <v>1.0049999999999999</v>
+        <v>1010</v>
       </c>
       <c r="F250" s="3">
-        <v>1.024</v>
+        <v>1020</v>
       </c>
       <c r="G250" s="3">
-        <v>1.03</v>
+        <v>1030</v>
       </c>
       <c r="H250" s="2" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.25">
@@ -7422,16 +7425,16 @@
         <v>70</v>
       </c>
       <c r="E251" s="3">
-        <v>1</v>
+        <v>1.0049999999999999</v>
       </c>
       <c r="F251" s="3">
-        <v>1.02</v>
+        <v>1.024</v>
       </c>
       <c r="G251" s="3">
-        <v>1.04</v>
+        <v>1.03</v>
       </c>
       <c r="H251" s="2" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.25">
@@ -7442,22 +7445,22 @@
         <v>54</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D252" s="1" t="s">
-        <v>33</v>
+        <v>55</v>
+      </c>
+      <c r="D252" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="E252" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F252" s="3">
-        <v>0</v>
+        <v>1.02</v>
       </c>
       <c r="G252" s="3">
-        <v>0</v>
+        <v>1.04</v>
       </c>
       <c r="H252" s="2" t="s">
-        <v>126</v>
+        <v>5</v>
       </c>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.25">
@@ -7483,7 +7486,7 @@
         <v>0</v>
       </c>
       <c r="H253" s="2" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.25">
@@ -7509,7 +7512,7 @@
         <v>0</v>
       </c>
       <c r="H254" s="2" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.25">
@@ -7520,7 +7523,7 @@
         <v>54</v>
       </c>
       <c r="C255" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D255" s="1" t="s">
         <v>33</v>
@@ -7535,7 +7538,7 @@
         <v>0</v>
       </c>
       <c r="H255" s="2" t="s">
-        <v>85</v>
+        <v>5</v>
       </c>
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.25">
@@ -7561,7 +7564,7 @@
         <v>0</v>
       </c>
       <c r="H256" s="2" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.25">
@@ -7572,7 +7575,7 @@
         <v>54</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="D257" s="1" t="s">
         <v>33</v>
@@ -7587,7 +7590,7 @@
         <v>0</v>
       </c>
       <c r="H257" s="2" t="s">
-        <v>85</v>
+        <v>5</v>
       </c>
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.25">
@@ -7613,7 +7616,7 @@
         <v>0</v>
       </c>
       <c r="H258" s="2" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.25">
@@ -7624,10 +7627,10 @@
         <v>54</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>140</v>
+        <v>84</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="E259" s="3">
         <v>0</v>
@@ -7639,7 +7642,7 @@
         <v>0</v>
       </c>
       <c r="H259" s="2" t="s">
-        <v>126</v>
+        <v>5</v>
       </c>
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.25">
@@ -7665,7 +7668,7 @@
         <v>0</v>
       </c>
       <c r="H260" s="2" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.25">
@@ -7691,7 +7694,7 @@
         <v>0</v>
       </c>
       <c r="H261" s="2" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.25">
@@ -7702,7 +7705,10 @@
         <v>54</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>57</v>
+        <v>140</v>
+      </c>
+      <c r="D262" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="E262" s="3">
         <v>0</v>
@@ -7714,7 +7720,7 @@
         <v>0</v>
       </c>
       <c r="H262" s="2" t="s">
-        <v>126</v>
+        <v>5</v>
       </c>
     </row>
     <row r="263" spans="1:8" x14ac:dyDescent="0.25">
@@ -7737,7 +7743,7 @@
         <v>0</v>
       </c>
       <c r="H263" s="2" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
     </row>
     <row r="264" spans="1:8" x14ac:dyDescent="0.25">
@@ -7760,7 +7766,7 @@
         <v>0</v>
       </c>
       <c r="H264" s="2" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="265" spans="1:8" x14ac:dyDescent="0.25">
@@ -7771,19 +7777,19 @@
         <v>54</v>
       </c>
       <c r="C265" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="E265" s="3">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="F265" s="3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G265" s="3">
-        <v>8.5</v>
+        <v>0</v>
       </c>
       <c r="H265" s="2" t="s">
-        <v>126</v>
+        <v>5</v>
       </c>
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.25">
@@ -7797,16 +7803,16 @@
         <v>83</v>
       </c>
       <c r="E266" s="3">
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
       <c r="F266" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="G266" s="3">
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
       <c r="H266" s="2" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.25">
@@ -7820,7 +7826,7 @@
         <v>83</v>
       </c>
       <c r="E267" s="3">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="F267" s="3">
         <v>5.5</v>
@@ -7829,7 +7835,7 @@
         <v>7.5</v>
       </c>
       <c r="H267" s="2" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.25">
@@ -7840,22 +7846,19 @@
         <v>54</v>
       </c>
       <c r="C268" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D268" s="1" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="E268" s="3">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="F268" s="3">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="G268" s="3">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="H268" s="2" t="s">
-        <v>85</v>
+        <v>5</v>
       </c>
     </row>
     <row r="269" spans="1:8" x14ac:dyDescent="0.25">
@@ -7866,7 +7869,7 @@
         <v>54</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>133</v>
+        <v>24</v>
       </c>
       <c r="D269" s="1" t="s">
         <v>33</v>
@@ -7907,7 +7910,7 @@
         <v>0</v>
       </c>
       <c r="H270" s="2" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.25">
@@ -7924,42 +7927,42 @@
         <v>33</v>
       </c>
       <c r="E271" s="3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F271" s="3">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G271" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H271" s="2" t="s">
-        <v>126</v>
+        <v>5</v>
       </c>
     </row>
     <row r="272" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>125</v>
+        <v>54</v>
       </c>
       <c r="C272" s="2" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>119</v>
+        <v>33</v>
       </c>
       <c r="E272" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F272" s="3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G272" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H272" s="2" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
     </row>
     <row r="273" spans="1:8" x14ac:dyDescent="0.25">
@@ -7970,19 +7973,19 @@
         <v>125</v>
       </c>
       <c r="C273" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D273" s="1" t="s">
-        <v>34</v>
+        <v>119</v>
       </c>
       <c r="E273" s="3">
         <v>0</v>
       </c>
       <c r="F273" s="3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G273" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H273" s="2" t="s">
         <v>111</v>
@@ -7996,22 +7999,22 @@
         <v>125</v>
       </c>
       <c r="C274" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>119</v>
+        <v>34</v>
       </c>
       <c r="E274" s="3">
         <v>0</v>
       </c>
       <c r="F274" s="3">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G274" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H274" s="2" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="275" spans="1:8" x14ac:dyDescent="0.25">
@@ -8037,7 +8040,7 @@
         <v>1</v>
       </c>
       <c r="H275" s="2" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.25">
@@ -8048,7 +8051,7 @@
         <v>125</v>
       </c>
       <c r="C276" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D276" s="1" t="s">
         <v>119</v>
@@ -8063,7 +8066,7 @@
         <v>1</v>
       </c>
       <c r="H276" s="2" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="277" spans="1:8" x14ac:dyDescent="0.25">
@@ -8089,7 +8092,7 @@
         <v>1</v>
       </c>
       <c r="H277" s="2" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
     </row>
     <row r="278" spans="1:8" x14ac:dyDescent="0.25">
@@ -8097,25 +8100,25 @@
         <v>60</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="C278" s="2" t="s">
-        <v>64</v>
+        <v>114</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>19</v>
+        <v>119</v>
       </c>
       <c r="E278" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F278" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G278" s="3">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="H278" s="2" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
     </row>
     <row r="279" spans="1:8" x14ac:dyDescent="0.25">
@@ -8135,13 +8138,13 @@
         <v>3</v>
       </c>
       <c r="F279" s="3">
-        <v>9.6</v>
+        <v>5</v>
       </c>
       <c r="G279" s="3">
         <v>17</v>
       </c>
       <c r="H279" s="2" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="280" spans="1:8" x14ac:dyDescent="0.25">
@@ -8152,22 +8155,22 @@
         <v>104</v>
       </c>
       <c r="C280" s="2" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="D280" s="1" t="s">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="E280" s="3">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="F280" s="3">
-        <v>116</v>
+        <v>9.6</v>
       </c>
       <c r="G280" s="3">
-        <v>158</v>
+        <v>17</v>
       </c>
       <c r="H280" s="2" t="s">
-        <v>91</v>
+        <v>5</v>
       </c>
     </row>
     <row r="281" spans="1:8" x14ac:dyDescent="0.25">
@@ -8178,22 +8181,22 @@
         <v>104</v>
       </c>
       <c r="C281" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="E281" s="3">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F281" s="3">
-        <v>20.5</v>
+        <v>116</v>
       </c>
       <c r="G281" s="3">
-        <v>96</v>
+        <v>158</v>
       </c>
       <c r="H281" s="2" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
     </row>
     <row r="282" spans="1:8" x14ac:dyDescent="0.25">
@@ -8210,16 +8213,16 @@
         <v>19</v>
       </c>
       <c r="E282" s="3">
-        <v>20.03</v>
+        <v>30</v>
       </c>
       <c r="F282" s="3">
-        <v>17.2258</v>
+        <v>20.5</v>
       </c>
       <c r="G282" s="3">
-        <v>60.09</v>
+        <v>96</v>
       </c>
       <c r="H282" s="2" t="s">
-        <v>111</v>
+        <v>5</v>
       </c>
     </row>
     <row r="283" spans="1:8" x14ac:dyDescent="0.25">
@@ -8239,13 +8242,13 @@
         <v>20.03</v>
       </c>
       <c r="F283" s="3">
-        <v>12.8192</v>
+        <v>17.2258</v>
       </c>
       <c r="G283" s="3">
         <v>60.09</v>
       </c>
       <c r="H283" s="2" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="284" spans="1:8" x14ac:dyDescent="0.25">
@@ -8256,22 +8259,22 @@
         <v>104</v>
       </c>
       <c r="C284" s="2" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="D284" s="1" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="E284" s="3">
-        <v>200</v>
+        <v>20.03</v>
       </c>
       <c r="F284" s="3">
-        <v>419</v>
+        <v>12.8192</v>
       </c>
       <c r="G284" s="3">
-        <v>950</v>
+        <v>60.09</v>
       </c>
       <c r="H284" s="2" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
     </row>
     <row r="285" spans="1:8" x14ac:dyDescent="0.25">
@@ -8288,16 +8291,16 @@
         <v>52</v>
       </c>
       <c r="E285" s="3">
-        <v>298.18799999999999</v>
+        <v>200</v>
       </c>
       <c r="F285" s="3">
-        <v>451.34819999999996</v>
-      </c>
-      <c r="G285" s="3" t="s">
-        <v>41</v>
+        <v>419</v>
+      </c>
+      <c r="G285" s="3">
+        <v>950</v>
       </c>
       <c r="H285" s="2" t="s">
-        <v>111</v>
+        <v>5</v>
       </c>
     </row>
     <row r="286" spans="1:8" x14ac:dyDescent="0.25">
@@ -8317,23 +8320,49 @@
         <v>298.18799999999999</v>
       </c>
       <c r="F286" s="3">
-        <v>356.47019999999998</v>
+        <v>451.34819999999996</v>
       </c>
       <c r="G286" s="3" t="s">
         <v>41</v>
       </c>
       <c r="H286" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A287" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B287" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C287" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D287" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E287" s="3">
+        <v>298.18799999999999</v>
+      </c>
+      <c r="F287" s="3">
+        <v>356.47019999999998</v>
+      </c>
+      <c r="G287" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H287" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H287" s="3"/>
     </row>
     <row r="288" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H288" s="3"/>
     </row>
     <row r="289" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H289" s="3"/>
+    </row>
+    <row r="290" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H290" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H1" xr:uid="{A46A3802-283E-4E98-BCAF-1BECEA2B901B}">
@@ -8342,7 +8371,7 @@
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="F1:F150 F152:F168 F170:F272 F279:F1048576">
+  <conditionalFormatting sqref="F153:F169 F171:F273 F280:F1048576 F1:F151">
     <cfRule type="cellIs" dxfId="6" priority="4" operator="notBetween">
       <formula>$E1</formula>
       <formula>$G1</formula>
@@ -8360,27 +8389,27 @@
       <formula>$G109</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F136:F138 F129 F142">
+  <conditionalFormatting sqref="F137:F139 F130 F143">
     <cfRule type="cellIs" dxfId="3" priority="25" operator="notBetween">
-      <formula>$G129</formula>
+      <formula>$G130</formula>
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F164 F151">
+  <conditionalFormatting sqref="F165 F152">
     <cfRule type="cellIs" dxfId="2" priority="33" operator="notBetween">
-      <formula>$G151</formula>
+      <formula>$G152</formula>
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H287:H289">
+  <conditionalFormatting sqref="H288:H290">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="notBetween">
-      <formula>$E287</formula>
-      <formula>$G287</formula>
+      <formula>$E288</formula>
+      <formula>$G288</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F169">
+  <conditionalFormatting sqref="F170">
     <cfRule type="cellIs" dxfId="0" priority="36" operator="notBetween">
-      <formula>$E169</formula>
+      <formula>$E170</formula>
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>